<commit_message>
RDM-9338: fixed failure test cases
</commit_message>
<xml_diff>
--- a/aat/src/resource/CCD_TestDefinition_Invalid_Case_Type_NOC_CONFIG.xlsx
+++ b/aat/src/resource/CCD_TestDefinition_Invalid_Case_Type_NOC_CONFIG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiranyenigala/Projects/CCD/ccd-definition-store-api/aat/src/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5568BF-7C80-7244-A833-B663ED975831}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C82BF5-62FE-3E42-BC50-43762CC62936}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35200" windowHeight="19700" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35200" windowHeight="19700" tabRatio="500" firstSheet="12" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="370">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -820,19 +820,10 @@
     <t>CRUD</t>
   </si>
   <si>
-    <t>CaseWorker1</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
-    <t>CaseWorker2</t>
-  </si>
-  <si>
     <t>C</t>
-  </si>
-  <si>
-    <t>CaseWorker3</t>
   </si>
   <si>
     <t>druc</t>
@@ -1193,6 +1184,9 @@
   </si>
   <si>
     <t>TestComplexAddressBookCase1</t>
+  </si>
+  <si>
+    <t>caseworker-test</t>
   </si>
 </sst>
 </file>
@@ -1204,7 +1198,7 @@
     <numFmt numFmtId="165" formatCode="d\/m\/yy"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="49" x14ac:knownFonts="1">
+  <fonts count="50" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1528,6 +1522,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1843,7 +1843,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="214">
+  <cellXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1998,7 +1998,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="7"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="14" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="26" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
@@ -2107,7 +2106,6 @@
     <xf numFmtId="14" fontId="26" fillId="0" borderId="0" xfId="8" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="8" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="9"/>
     <xf numFmtId="49" fontId="42" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2144,6 +2142,7 @@
     <xf numFmtId="49" fontId="48" fillId="4" borderId="21" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -3118,9 +3117,9 @@
         <v>185</v>
       </c>
       <c r="K2" s="100" t="s">
-        <v>264</v>
-      </c>
-      <c r="L2" s="152"/>
+        <v>261</v>
+      </c>
+      <c r="L2" s="151"/>
       <c r="M2" s="13" t="s">
         <v>116</v>
       </c>
@@ -3131,7 +3130,7 @@
         <v>187</v>
       </c>
       <c r="P2" s="102" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -3168,10 +3167,10 @@
         <v>194</v>
       </c>
       <c r="K3" s="101" t="s">
-        <v>265</v>
-      </c>
-      <c r="L3" s="153" t="s">
-        <v>315</v>
+        <v>262</v>
+      </c>
+      <c r="L3" s="152" t="s">
+        <v>312</v>
       </c>
       <c r="M3" s="7" t="s">
         <v>118</v>
@@ -3183,13 +3182,13 @@
         <v>197</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="Q3" s="151" t="s">
-        <v>309</v>
-      </c>
-      <c r="R3" s="151" t="s">
-        <v>310</v>
+        <v>270</v>
+      </c>
+      <c r="Q3" s="150" t="s">
+        <v>306</v>
+      </c>
+      <c r="R3" s="150" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3220,7 +3219,7 @@
         <v>1</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="L4" s="99"/>
       <c r="M4" s="4"/>
@@ -3232,10 +3231,10 @@
         <v>2</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3266,7 +3265,7 @@
         <v>2</v>
       </c>
       <c r="K5" s="99" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="L5" s="99"/>
       <c r="M5" s="4"/>
@@ -3306,7 +3305,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="99" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="L6" s="99"/>
       <c r="M6" s="4"/>
@@ -3342,7 +3341,7 @@
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="99" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="L7" s="99"/>
       <c r="M7" s="4"/>
@@ -3378,7 +3377,7 @@
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="99" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="L8" s="99"/>
       <c r="M8" s="3" t="s">
@@ -3418,7 +3417,7 @@
         <v>1</v>
       </c>
       <c r="K9" s="99" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="L9" s="99"/>
       <c r="M9" s="4"/>
@@ -3450,7 +3449,7 @@
       </c>
       <c r="H10" s="113"/>
       <c r="I10" s="111" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="J10" s="113">
         <v>1</v>
@@ -3490,13 +3489,13 @@
       </c>
       <c r="H11" s="113"/>
       <c r="I11" s="33" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J11" s="113">
         <v>1</v>
       </c>
       <c r="K11" s="113" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="L11" s="113"/>
       <c r="M11" s="113"/>
@@ -3530,13 +3529,13 @@
       </c>
       <c r="H12" s="113"/>
       <c r="I12" s="33" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="J12" s="113">
         <v>1</v>
       </c>
       <c r="K12" s="113" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="L12" s="113"/>
       <c r="M12" s="113"/>
@@ -3588,10 +3587,10 @@
       </c>
       <c r="P13" s="4"/>
       <c r="Q13" s="4" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3624,7 +3623,7 @@
         <v>2</v>
       </c>
       <c r="K14" s="99" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="L14" s="99"/>
       <c r="M14" s="4"/>
@@ -3652,23 +3651,23 @@
       <c r="E15" s="111" t="s">
         <v>202</v>
       </c>
-      <c r="F15" s="117" t="s">
-        <v>317</v>
+      <c r="F15" s="116" t="s">
+        <v>314</v>
       </c>
       <c r="G15" s="4">
         <v>1</v>
       </c>
       <c r="H15" s="4"/>
-      <c r="I15" s="117" t="s">
-        <v>316</v>
+      <c r="I15" s="116" t="s">
+        <v>313</v>
       </c>
       <c r="J15" s="4">
         <v>1</v>
       </c>
       <c r="K15" s="99" t="s">
-        <v>267</v>
-      </c>
-      <c r="L15" s="155"/>
+        <v>264</v>
+      </c>
+      <c r="L15" s="154"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
@@ -3704,7 +3703,7 @@
         <v>1</v>
       </c>
       <c r="K16" s="99" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="L16" s="99"/>
       <c r="M16" s="4"/>
@@ -3722,13 +3721,13 @@
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="111"/>
-      <c r="F17" s="117"/>
+      <c r="F17" s="116"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
-      <c r="I17" s="117"/>
+      <c r="I17" s="116"/>
       <c r="J17" s="4"/>
       <c r="K17" s="99"/>
-      <c r="L17" s="154"/>
+      <c r="L17" s="153"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
@@ -3830,7 +3829,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F3"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3858,8 +3857,8 @@
         <v>3</v>
       </c>
       <c r="E1" s="47"/>
-      <c r="F1" s="177"/>
-      <c r="G1" s="177"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
       <c r="H1" s="47"/>
     </row>
     <row r="2" spans="1:8" ht="80" x14ac:dyDescent="0.15">
@@ -3874,11 +3873,11 @@
       <c r="E2" s="49" t="s">
         <v>215</v>
       </c>
-      <c r="F2" s="205" t="s">
-        <v>362</v>
-      </c>
-      <c r="G2" s="165" t="s">
-        <v>331</v>
+      <c r="F2" s="203" t="s">
+        <v>359</v>
+      </c>
+      <c r="G2" s="164" t="s">
+        <v>328</v>
       </c>
       <c r="H2" s="49" t="s">
         <v>156</v>
@@ -3900,10 +3899,10 @@
       <c r="E3" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="161" t="s">
+      <c r="F3" s="160" t="s">
         <v>118</v>
       </c>
-      <c r="G3" s="124" t="s">
+      <c r="G3" s="123" t="s">
         <v>247</v>
       </c>
       <c r="H3" s="50" t="s">
@@ -3924,8 +3923,8 @@
       <c r="E4" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="172"/>
-      <c r="G4" s="172"/>
+      <c r="F4" s="171"/>
+      <c r="G4" s="171"/>
       <c r="H4" s="47">
         <v>1</v>
       </c>
@@ -3944,8 +3943,8 @@
       <c r="E5" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="172"/>
-      <c r="G5" s="172"/>
+      <c r="F5" s="171"/>
+      <c r="G5" s="171"/>
       <c r="H5" s="47">
         <v>2</v>
       </c>
@@ -3964,8 +3963,8 @@
       <c r="E6" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="172"/>
-      <c r="G6" s="172"/>
+      <c r="F6" s="171"/>
+      <c r="G6" s="171"/>
       <c r="H6" s="47">
         <v>3</v>
       </c>
@@ -3984,9 +3983,9 @@
       <c r="E7" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="172"/>
-      <c r="G7" s="172" t="s">
-        <v>249</v>
+      <c r="F7" s="171"/>
+      <c r="G7" s="212" t="s">
+        <v>369</v>
       </c>
       <c r="H7" s="47">
         <v>1</v>
@@ -4006,8 +4005,8 @@
       <c r="E8" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="172"/>
-      <c r="G8" s="172"/>
+      <c r="F8" s="171"/>
+      <c r="G8" s="171"/>
       <c r="H8" s="47">
         <v>2</v>
       </c>
@@ -4026,8 +4025,8 @@
       <c r="E9" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="F9" s="172"/>
-      <c r="G9" s="172"/>
+      <c r="F9" s="171"/>
+      <c r="G9" s="171"/>
       <c r="H9" s="47">
         <v>3</v>
       </c>
@@ -4046,8 +4045,8 @@
       <c r="E10" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="F10" s="172"/>
-      <c r="G10" s="172"/>
+      <c r="F10" s="171"/>
+      <c r="G10" s="171"/>
       <c r="H10" s="47">
         <v>4</v>
       </c>
@@ -4066,8 +4065,8 @@
       <c r="E11" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="F11" s="172"/>
-      <c r="G11" s="172"/>
+      <c r="F11" s="171"/>
+      <c r="G11" s="171"/>
       <c r="H11" s="47">
         <v>5</v>
       </c>
@@ -4086,8 +4085,8 @@
       <c r="E12" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="F12" s="172"/>
-      <c r="G12" s="172"/>
+      <c r="F12" s="171"/>
+      <c r="G12" s="171"/>
       <c r="H12" s="47">
         <v>6</v>
       </c>
@@ -4106,8 +4105,8 @@
       <c r="E13" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="172"/>
-      <c r="G13" s="172"/>
+      <c r="F13" s="171"/>
+      <c r="G13" s="171"/>
       <c r="H13" s="47">
         <v>7</v>
       </c>
@@ -4126,8 +4125,8 @@
       <c r="E14" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="F14" s="172"/>
-      <c r="G14" s="172"/>
+      <c r="F14" s="171"/>
+      <c r="G14" s="171"/>
       <c r="H14" s="47">
         <v>8</v>
       </c>
@@ -4146,8 +4145,8 @@
       <c r="E15" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="F15" s="172"/>
-      <c r="G15" s="172"/>
+      <c r="F15" s="171"/>
+      <c r="G15" s="171"/>
       <c r="H15" s="47">
         <v>9</v>
       </c>
@@ -4166,10 +4165,10 @@
       <c r="E16" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="F16" s="172" t="s">
-        <v>363</v>
-      </c>
-      <c r="G16" s="172"/>
+      <c r="F16" s="171" t="s">
+        <v>360</v>
+      </c>
+      <c r="G16" s="171"/>
       <c r="H16" s="47">
         <v>10</v>
       </c>
@@ -4188,7 +4187,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4231,8 +4230,8 @@
       <c r="E2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="165" t="s">
-        <v>331</v>
+      <c r="F2" s="164" t="s">
+        <v>328</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>156</v>
@@ -4254,7 +4253,7 @@
       <c r="E3" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="124" t="s">
+      <c r="F3" s="123" t="s">
         <v>247</v>
       </c>
       <c r="G3" s="7" t="s">
@@ -4275,7 +4274,7 @@
       <c r="E4" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="172"/>
+      <c r="F4" s="171"/>
       <c r="G4" s="47">
         <v>1</v>
       </c>
@@ -4294,7 +4293,7 @@
       <c r="E5" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="172"/>
+      <c r="F5" s="171"/>
       <c r="G5" s="47">
         <v>2</v>
       </c>
@@ -4313,27 +4312,27 @@
       <c r="E6" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="172"/>
+      <c r="F6" s="171"/>
       <c r="G6" s="47">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="202">
-        <v>42736</v>
-      </c>
-      <c r="B7" s="203"/>
-      <c r="C7" s="178" t="s">
+      <c r="A7" s="200">
+        <v>42736</v>
+      </c>
+      <c r="B7" s="201"/>
+      <c r="C7" s="177" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="178" t="s">
-        <v>360</v>
-      </c>
-      <c r="E7" s="204" t="s">
-        <v>361</v>
-      </c>
-      <c r="F7" s="204"/>
-      <c r="G7" s="203">
+      <c r="D7" s="177" t="s">
+        <v>357</v>
+      </c>
+      <c r="E7" s="202" t="s">
+        <v>358</v>
+      </c>
+      <c r="F7" s="202"/>
+      <c r="G7" s="201">
         <v>4</v>
       </c>
     </row>
@@ -4351,8 +4350,8 @@
       <c r="E8" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="F8" s="172" t="s">
-        <v>249</v>
+      <c r="F8" s="212" t="s">
+        <v>369</v>
       </c>
       <c r="G8" s="47">
         <v>2</v>
@@ -4372,7 +4371,7 @@
       <c r="E9" s="53" t="s">
         <v>218</v>
       </c>
-      <c r="F9" s="172"/>
+      <c r="F9" s="171"/>
       <c r="G9" s="47">
         <v>3</v>
       </c>
@@ -4391,7 +4390,7 @@
       <c r="E10" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="172"/>
+      <c r="F10" s="171"/>
       <c r="G10" s="47">
         <v>1</v>
       </c>
@@ -4410,7 +4409,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G1"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -4438,7 +4437,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="60"/>
-      <c r="F1" s="177"/>
+      <c r="F1" s="176"/>
       <c r="G1" s="60"/>
       <c r="H1" s="60"/>
     </row>
@@ -4454,11 +4453,11 @@
       <c r="E2" s="62" t="s">
         <v>222</v>
       </c>
-      <c r="F2" s="205" t="s">
-        <v>362</v>
-      </c>
-      <c r="G2" s="165" t="s">
-        <v>331</v>
+      <c r="F2" s="203" t="s">
+        <v>359</v>
+      </c>
+      <c r="G2" s="164" t="s">
+        <v>328</v>
       </c>
       <c r="H2" s="62" t="s">
         <v>156</v>
@@ -4480,10 +4479,10 @@
       <c r="E3" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="161" t="s">
+      <c r="F3" s="160" t="s">
         <v>118</v>
       </c>
-      <c r="G3" s="124" t="s">
+      <c r="G3" s="123" t="s">
         <v>247</v>
       </c>
       <c r="H3" s="63" t="s">
@@ -4504,8 +4503,8 @@
       <c r="E4" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="172"/>
-      <c r="G4" s="172"/>
+      <c r="F4" s="171"/>
+      <c r="G4" s="171"/>
       <c r="H4" s="47">
         <v>1</v>
       </c>
@@ -4525,7 +4524,7 @@
         <v>53</v>
       </c>
       <c r="F5" s="53"/>
-      <c r="G5" s="172"/>
+      <c r="G5" s="171"/>
       <c r="H5" s="47">
         <v>2</v>
       </c>
@@ -4544,8 +4543,8 @@
       <c r="E6" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="172"/>
-      <c r="G6" s="172"/>
+      <c r="F6" s="171"/>
+      <c r="G6" s="171"/>
       <c r="H6" s="47">
         <v>3</v>
       </c>
@@ -4564,9 +4563,9 @@
       <c r="E7" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="172"/>
-      <c r="G7" s="172" t="s">
-        <v>249</v>
+      <c r="F7" s="171"/>
+      <c r="G7" s="212" t="s">
+        <v>369</v>
       </c>
       <c r="H7" s="47">
         <v>1</v>
@@ -4586,8 +4585,8 @@
       <c r="E8" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="172"/>
-      <c r="G8" s="172"/>
+      <c r="F8" s="171"/>
+      <c r="G8" s="171"/>
       <c r="H8" s="47">
         <v>2</v>
       </c>
@@ -4606,8 +4605,8 @@
       <c r="E9" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="F9" s="172"/>
-      <c r="G9" s="172"/>
+      <c r="F9" s="171"/>
+      <c r="G9" s="171"/>
       <c r="H9" s="47">
         <v>3</v>
       </c>
@@ -4626,8 +4625,8 @@
       <c r="E10" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="F10" s="172"/>
-      <c r="G10" s="172"/>
+      <c r="F10" s="171"/>
+      <c r="G10" s="171"/>
       <c r="H10" s="47">
         <v>4</v>
       </c>
@@ -4646,8 +4645,8 @@
       <c r="E11" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="F11" s="172"/>
-      <c r="G11" s="172"/>
+      <c r="F11" s="171"/>
+      <c r="G11" s="171"/>
       <c r="H11" s="47">
         <v>5</v>
       </c>
@@ -4666,8 +4665,8 @@
       <c r="E12" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="F12" s="172"/>
-      <c r="G12" s="172"/>
+      <c r="F12" s="171"/>
+      <c r="G12" s="171"/>
       <c r="H12" s="47">
         <v>6</v>
       </c>
@@ -4686,8 +4685,8 @@
       <c r="E13" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="172"/>
-      <c r="G13" s="172"/>
+      <c r="F13" s="171"/>
+      <c r="G13" s="171"/>
       <c r="H13" s="47">
         <v>7</v>
       </c>
@@ -4707,9 +4706,9 @@
         <v>82</v>
       </c>
       <c r="F14" s="53" t="s">
-        <v>364</v>
-      </c>
-      <c r="G14" s="172"/>
+        <v>361</v>
+      </c>
+      <c r="G14" s="171"/>
       <c r="H14" s="47">
         <v>8</v>
       </c>
@@ -4728,8 +4727,8 @@
       <c r="E15" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="F15" s="172"/>
-      <c r="G15" s="172"/>
+      <c r="F15" s="171"/>
+      <c r="G15" s="171"/>
       <c r="H15" s="47">
         <v>9</v>
       </c>
@@ -4748,8 +4747,8 @@
       <c r="E16" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="F16" s="172"/>
-      <c r="G16" s="172"/>
+      <c r="F16" s="171"/>
+      <c r="G16" s="171"/>
       <c r="H16" s="47">
         <v>10</v>
       </c>
@@ -4811,8 +4810,8 @@
       <c r="E2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="165" t="s">
-        <v>331</v>
+      <c r="F2" s="164" t="s">
+        <v>328</v>
       </c>
       <c r="G2" s="64" t="s">
         <v>156</v>
@@ -4834,7 +4833,7 @@
       <c r="E3" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="124" t="s">
+      <c r="F3" s="123" t="s">
         <v>247</v>
       </c>
       <c r="G3" s="7" t="s">
@@ -4855,7 +4854,7 @@
       <c r="E4" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="172"/>
+      <c r="F4" s="171"/>
       <c r="G4" s="47">
         <v>1</v>
       </c>
@@ -4874,7 +4873,7 @@
       <c r="E5" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="172"/>
+      <c r="F5" s="171"/>
       <c r="G5" s="47">
         <v>1</v>
       </c>
@@ -4893,7 +4892,7 @@
       <c r="E6" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="172"/>
+      <c r="F6" s="171"/>
       <c r="G6" s="47">
         <v>1</v>
       </c>
@@ -4903,7 +4902,7 @@
         <v>42736</v>
       </c>
       <c r="B7" s="47"/>
-      <c r="C7" s="117" t="s">
+      <c r="C7" s="116" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -4912,8 +4911,8 @@
       <c r="E7" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F7" s="119" t="s">
-        <v>249</v>
+      <c r="F7" s="212" t="s">
+        <v>369</v>
       </c>
       <c r="G7" s="47">
         <v>2</v>
@@ -4933,7 +4932,7 @@
       <c r="E8" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F8" s="119"/>
+      <c r="F8" s="118"/>
       <c r="G8" s="47">
         <v>3</v>
       </c>
@@ -4952,7 +4951,7 @@
       <c r="E9" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="172"/>
+      <c r="F9" s="171"/>
       <c r="G9" s="47">
         <v>1</v>
       </c>
@@ -4971,7 +4970,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="G1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4997,13 +4996,13 @@
         <v>224</v>
       </c>
       <c r="B1" s="4"/>
-      <c r="C1" s="174" t="s">
+      <c r="C1" s="173" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="175" t="s">
+      <c r="D1" s="174" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="176" t="s">
+      <c r="E1" s="175" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="4"/>
@@ -5016,174 +5015,174 @@
       <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:13" ht="70" x14ac:dyDescent="0.15">
-      <c r="A2" s="166"/>
-      <c r="B2" s="166"/>
-      <c r="C2" s="165" t="s">
+      <c r="A2" s="165"/>
+      <c r="B2" s="165"/>
+      <c r="C2" s="164" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="165" t="s">
+      <c r="D2" s="164" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="165" t="s">
+      <c r="E2" s="164" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="164" t="s">
+      <c r="F2" s="163" t="s">
         <v>225</v>
       </c>
-      <c r="G2" s="164" t="s">
+      <c r="G2" s="163" t="s">
         <v>226</v>
       </c>
-      <c r="H2" s="164" t="s">
+      <c r="H2" s="163" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="165" t="s">
-        <v>331</v>
-      </c>
-      <c r="J2" s="164" t="s">
+      <c r="I2" s="164" t="s">
+        <v>328</v>
+      </c>
+      <c r="J2" s="163" t="s">
         <v>226</v>
       </c>
-      <c r="K2" s="160" t="s">
-        <v>272</v>
-      </c>
-      <c r="L2" s="167" t="s">
-        <v>271</v>
-      </c>
-      <c r="M2" s="168" t="s">
-        <v>318</v>
+      <c r="K2" s="159" t="s">
+        <v>269</v>
+      </c>
+      <c r="L2" s="166" t="s">
+        <v>268</v>
+      </c>
+      <c r="M2" s="167" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="124" t="s">
+      <c r="A3" s="123" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="124" t="s">
+      <c r="B3" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="124" t="s">
+      <c r="C3" s="123" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="124" t="s">
+      <c r="D3" s="123" t="s">
         <v>227</v>
       </c>
-      <c r="E3" s="124" t="s">
+      <c r="E3" s="123" t="s">
         <v>228</v>
       </c>
-      <c r="F3" s="124" t="s">
+      <c r="F3" s="123" t="s">
         <v>229</v>
       </c>
-      <c r="G3" s="124" t="s">
+      <c r="G3" s="123" t="s">
         <v>230</v>
       </c>
-      <c r="H3" s="124" t="s">
+      <c r="H3" s="123" t="s">
         <v>193</v>
       </c>
-      <c r="I3" s="124" t="s">
+      <c r="I3" s="123" t="s">
         <v>247</v>
       </c>
-      <c r="J3" s="124" t="s">
+      <c r="J3" s="123" t="s">
         <v>231</v>
       </c>
-      <c r="K3" s="169" t="s">
+      <c r="K3" s="168" t="s">
         <v>118</v>
       </c>
-      <c r="L3" s="169" t="s">
-        <v>268</v>
-      </c>
-      <c r="M3" s="170" t="s">
-        <v>315</v>
+      <c r="L3" s="168" t="s">
+        <v>265</v>
+      </c>
+      <c r="M3" s="169" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="171">
-        <v>42736</v>
-      </c>
-      <c r="B4" s="171"/>
-      <c r="C4" s="119" t="s">
+      <c r="A4" s="170">
+        <v>42736</v>
+      </c>
+      <c r="B4" s="170"/>
+      <c r="C4" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="119" t="s">
+      <c r="D4" s="118" t="s">
         <v>232</v>
       </c>
-      <c r="E4" s="119" t="s">
+      <c r="E4" s="118" t="s">
         <v>233</v>
       </c>
-      <c r="F4" s="172" t="s">
+      <c r="F4" s="171" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="99">
         <v>1</v>
       </c>
-      <c r="H4" s="119" t="s">
+      <c r="H4" s="118" t="s">
         <v>45</v>
       </c>
       <c r="J4" s="99">
         <v>1</v>
       </c>
-      <c r="K4" s="163"/>
-      <c r="L4" s="163" t="s">
-        <v>270</v>
+      <c r="K4" s="162"/>
+      <c r="L4" s="162" t="s">
+        <v>267</v>
       </c>
       <c r="M4" s="107"/>
     </row>
     <row r="5" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="171">
-        <v>42736</v>
-      </c>
-      <c r="B5" s="171"/>
-      <c r="C5" s="119" t="s">
+      <c r="A5" s="170">
+        <v>42736</v>
+      </c>
+      <c r="B5" s="170"/>
+      <c r="C5" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="119" t="s">
+      <c r="D5" s="118" t="s">
         <v>232</v>
       </c>
-      <c r="E5" s="119" t="s">
+      <c r="E5" s="118" t="s">
         <v>233</v>
       </c>
-      <c r="F5" s="172" t="s">
+      <c r="F5" s="171" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="99">
         <v>1</v>
       </c>
-      <c r="H5" s="119" t="s">
+      <c r="H5" s="118" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="150" t="s">
-        <v>249</v>
+      <c r="I5" s="212" t="s">
+        <v>369</v>
       </c>
       <c r="J5" s="99">
         <v>2</v>
       </c>
-      <c r="K5" s="119" t="s">
-        <v>269</v>
-      </c>
-      <c r="L5" s="163"/>
+      <c r="K5" s="118" t="s">
+        <v>266</v>
+      </c>
+      <c r="L5" s="162"/>
       <c r="M5" s="99"/>
     </row>
     <row r="6" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="171">
-        <v>42736</v>
-      </c>
-      <c r="B6" s="171"/>
-      <c r="C6" s="119" t="s">
+      <c r="A6" s="170">
+        <v>42736</v>
+      </c>
+      <c r="B6" s="170"/>
+      <c r="C6" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="119" t="s">
+      <c r="D6" s="118" t="s">
         <v>232</v>
       </c>
-      <c r="E6" s="119" t="s">
+      <c r="E6" s="118" t="s">
         <v>234</v>
       </c>
-      <c r="F6" s="172" t="s">
+      <c r="F6" s="171" t="s">
         <v>55</v>
       </c>
       <c r="G6" s="99">
         <v>2</v>
       </c>
-      <c r="H6" s="119" t="s">
+      <c r="H6" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="I6" s="119"/>
+      <c r="I6" s="118"/>
       <c r="J6" s="99">
         <v>1</v>
       </c>
@@ -5192,29 +5191,29 @@
       <c r="M6" s="99"/>
     </row>
     <row r="7" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="171">
-        <v>42736</v>
-      </c>
-      <c r="B7" s="171"/>
-      <c r="C7" s="119" t="s">
+      <c r="A7" s="170">
+        <v>42736</v>
+      </c>
+      <c r="B7" s="170"/>
+      <c r="C7" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="119" t="s">
+      <c r="D7" s="118" t="s">
         <v>232</v>
       </c>
-      <c r="E7" s="119" t="s">
-        <v>284</v>
-      </c>
-      <c r="F7" s="172" t="s">
-        <v>285</v>
+      <c r="E7" s="118" t="s">
+        <v>281</v>
+      </c>
+      <c r="F7" s="171" t="s">
+        <v>282</v>
       </c>
       <c r="G7" s="99">
         <v>3</v>
       </c>
-      <c r="H7" s="119" t="s">
-        <v>282</v>
-      </c>
-      <c r="I7" s="119"/>
+      <c r="H7" s="118" t="s">
+        <v>279</v>
+      </c>
+      <c r="I7" s="118"/>
       <c r="J7" s="99">
         <v>1</v>
       </c>
@@ -5223,29 +5222,29 @@
       <c r="M7" s="99"/>
     </row>
     <row r="8" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="171">
-        <v>42736</v>
-      </c>
-      <c r="B8" s="171"/>
-      <c r="C8" s="119" t="s">
+      <c r="A8" s="170">
+        <v>42736</v>
+      </c>
+      <c r="B8" s="170"/>
+      <c r="C8" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="119" t="s">
+      <c r="D8" s="118" t="s">
         <v>232</v>
       </c>
-      <c r="E8" s="119" t="s">
-        <v>329</v>
-      </c>
-      <c r="F8" s="172" t="s">
-        <v>330</v>
+      <c r="E8" s="118" t="s">
+        <v>326</v>
+      </c>
+      <c r="F8" s="171" t="s">
+        <v>327</v>
       </c>
       <c r="G8" s="99">
         <v>4</v>
       </c>
-      <c r="H8" s="119" t="s">
-        <v>327</v>
-      </c>
-      <c r="I8" s="119"/>
+      <c r="H8" s="118" t="s">
+        <v>324</v>
+      </c>
+      <c r="I8" s="118"/>
       <c r="J8" s="99">
         <v>1</v>
       </c>
@@ -5254,60 +5253,60 @@
       <c r="M8" s="99"/>
     </row>
     <row r="9" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="171">
-        <v>42736</v>
-      </c>
-      <c r="B9" s="171"/>
-      <c r="C9" s="119" t="s">
+      <c r="A9" s="170">
+        <v>42736</v>
+      </c>
+      <c r="B9" s="170"/>
+      <c r="C9" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="119" t="s">
+      <c r="D9" s="118" t="s">
         <v>232</v>
       </c>
-      <c r="E9" s="150" t="s">
-        <v>319</v>
-      </c>
-      <c r="F9" s="172" t="s">
-        <v>317</v>
+      <c r="E9" s="149" t="s">
+        <v>316</v>
+      </c>
+      <c r="F9" s="171" t="s">
+        <v>314</v>
       </c>
       <c r="G9" s="99">
         <v>4</v>
       </c>
-      <c r="H9" s="150" t="s">
-        <v>316</v>
-      </c>
-      <c r="I9" s="150"/>
+      <c r="H9" s="149" t="s">
+        <v>313</v>
+      </c>
+      <c r="I9" s="149"/>
       <c r="J9" s="99">
         <v>1</v>
       </c>
       <c r="K9" s="99"/>
       <c r="L9" s="99"/>
-      <c r="M9" s="173"/>
+      <c r="M9" s="172"/>
     </row>
     <row r="10" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="171">
-        <v>42736</v>
-      </c>
-      <c r="B10" s="171"/>
-      <c r="C10" s="119" t="s">
+      <c r="A10" s="170">
+        <v>42736</v>
+      </c>
+      <c r="B10" s="170"/>
+      <c r="C10" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="119" t="s">
+      <c r="D10" s="118" t="s">
         <v>232</v>
       </c>
-      <c r="E10" s="119" t="s">
+      <c r="E10" s="118" t="s">
         <v>233</v>
       </c>
-      <c r="F10" s="172" t="s">
+      <c r="F10" s="171" t="s">
         <v>10</v>
       </c>
       <c r="G10" s="99">
         <v>1</v>
       </c>
-      <c r="H10" s="119" t="s">
+      <c r="H10" s="118" t="s">
         <v>45</v>
       </c>
-      <c r="I10" s="150"/>
+      <c r="I10" s="149"/>
       <c r="J10" s="99">
         <v>1</v>
       </c>
@@ -5316,29 +5315,29 @@
       <c r="M10" s="99"/>
     </row>
     <row r="11" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="171">
-        <v>42736</v>
-      </c>
-      <c r="B11" s="171"/>
-      <c r="C11" s="119" t="s">
+      <c r="A11" s="170">
+        <v>42736</v>
+      </c>
+      <c r="B11" s="170"/>
+      <c r="C11" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="119" t="s">
+      <c r="D11" s="118" t="s">
         <v>232</v>
       </c>
-      <c r="E11" s="119" t="s">
+      <c r="E11" s="118" t="s">
         <v>233</v>
       </c>
-      <c r="F11" s="172" t="s">
+      <c r="F11" s="171" t="s">
         <v>10</v>
       </c>
       <c r="G11" s="99">
         <v>1</v>
       </c>
-      <c r="H11" s="119" t="s">
+      <c r="H11" s="118" t="s">
         <v>52</v>
       </c>
-      <c r="I11" s="119"/>
+      <c r="I11" s="118"/>
       <c r="J11" s="99">
         <v>2</v>
       </c>
@@ -5347,29 +5346,29 @@
       <c r="M11" s="99"/>
     </row>
     <row r="12" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="171">
-        <v>42736</v>
-      </c>
-      <c r="B12" s="171"/>
-      <c r="C12" s="119" t="s">
+      <c r="A12" s="170">
+        <v>42736</v>
+      </c>
+      <c r="B12" s="170"/>
+      <c r="C12" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="119" t="s">
+      <c r="D12" s="118" t="s">
         <v>232</v>
       </c>
-      <c r="E12" s="119" t="s">
+      <c r="E12" s="118" t="s">
         <v>234</v>
       </c>
-      <c r="F12" s="172" t="s">
+      <c r="F12" s="171" t="s">
         <v>55</v>
       </c>
       <c r="G12" s="99">
         <v>2</v>
       </c>
-      <c r="H12" s="119" t="s">
+      <c r="H12" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="I12" s="119"/>
+      <c r="I12" s="118"/>
       <c r="J12" s="99">
         <v>1</v>
       </c>
@@ -5378,29 +5377,29 @@
       <c r="M12" s="99"/>
     </row>
     <row r="13" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="171">
-        <v>42736</v>
-      </c>
-      <c r="B13" s="171"/>
-      <c r="C13" s="119" t="s">
+      <c r="A13" s="170">
+        <v>42736</v>
+      </c>
+      <c r="B13" s="170"/>
+      <c r="C13" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="119" t="s">
+      <c r="D13" s="118" t="s">
         <v>232</v>
       </c>
-      <c r="E13" s="119" t="s">
+      <c r="E13" s="118" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="172" t="s">
+      <c r="F13" s="171" t="s">
         <v>235</v>
       </c>
       <c r="G13" s="99">
         <v>3</v>
       </c>
-      <c r="H13" s="119" t="s">
+      <c r="H13" s="118" t="s">
         <v>71</v>
       </c>
-      <c r="I13" s="119"/>
+      <c r="I13" s="118"/>
       <c r="J13" s="99">
         <v>1</v>
       </c>
@@ -5409,29 +5408,29 @@
       <c r="M13" s="99"/>
     </row>
     <row r="14" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="171">
-        <v>42736</v>
-      </c>
-      <c r="B14" s="171"/>
-      <c r="C14" s="119" t="s">
+      <c r="A14" s="170">
+        <v>42736</v>
+      </c>
+      <c r="B14" s="170"/>
+      <c r="C14" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="119" t="s">
+      <c r="D14" s="118" t="s">
         <v>232</v>
       </c>
-      <c r="E14" s="119" t="s">
+      <c r="E14" s="118" t="s">
         <v>74</v>
       </c>
-      <c r="F14" s="172" t="s">
+      <c r="F14" s="171" t="s">
         <v>235</v>
       </c>
       <c r="G14" s="99">
         <v>3</v>
       </c>
-      <c r="H14" s="119" t="s">
+      <c r="H14" s="118" t="s">
         <v>74</v>
       </c>
-      <c r="I14" s="119"/>
+      <c r="I14" s="118"/>
       <c r="J14" s="99">
         <v>2</v>
       </c>
@@ -5440,29 +5439,29 @@
       <c r="M14" s="99"/>
     </row>
     <row r="15" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="171">
-        <v>42736</v>
-      </c>
-      <c r="B15" s="171"/>
-      <c r="C15" s="119" t="s">
+      <c r="A15" s="170">
+        <v>42736</v>
+      </c>
+      <c r="B15" s="170"/>
+      <c r="C15" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="119" t="s">
+      <c r="D15" s="118" t="s">
         <v>232</v>
       </c>
-      <c r="E15" s="119" t="s">
+      <c r="E15" s="118" t="s">
         <v>77</v>
       </c>
-      <c r="F15" s="172" t="s">
+      <c r="F15" s="171" t="s">
         <v>235</v>
       </c>
       <c r="G15" s="99">
         <v>3</v>
       </c>
-      <c r="H15" s="119" t="s">
+      <c r="H15" s="118" t="s">
         <v>77</v>
       </c>
-      <c r="I15" s="119"/>
+      <c r="I15" s="118"/>
       <c r="J15" s="99">
         <v>3</v>
       </c>
@@ -5471,29 +5470,29 @@
       <c r="M15" s="99"/>
     </row>
     <row r="16" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="171">
-        <v>42736</v>
-      </c>
-      <c r="B16" s="171"/>
-      <c r="C16" s="119" t="s">
+      <c r="A16" s="170">
+        <v>42736</v>
+      </c>
+      <c r="B16" s="170"/>
+      <c r="C16" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="119" t="s">
+      <c r="D16" s="118" t="s">
         <v>232</v>
       </c>
-      <c r="E16" s="119" t="s">
+      <c r="E16" s="118" t="s">
         <v>79</v>
       </c>
-      <c r="F16" s="172" t="s">
+      <c r="F16" s="171" t="s">
         <v>236</v>
       </c>
       <c r="G16" s="99">
         <v>4</v>
       </c>
-      <c r="H16" s="119" t="s">
+      <c r="H16" s="118" t="s">
         <v>79</v>
       </c>
-      <c r="I16" s="119"/>
+      <c r="I16" s="118"/>
       <c r="J16" s="99">
         <v>1</v>
       </c>
@@ -5502,29 +5501,29 @@
       <c r="M16" s="99"/>
     </row>
     <row r="17" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="171">
-        <v>42736</v>
-      </c>
-      <c r="B17" s="171"/>
-      <c r="C17" s="119" t="s">
+      <c r="A17" s="170">
+        <v>42736</v>
+      </c>
+      <c r="B17" s="170"/>
+      <c r="C17" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="119" t="s">
+      <c r="D17" s="118" t="s">
         <v>232</v>
       </c>
-      <c r="E17" s="119" t="s">
+      <c r="E17" s="118" t="s">
         <v>81</v>
       </c>
-      <c r="F17" s="172" t="s">
+      <c r="F17" s="171" t="s">
         <v>235</v>
       </c>
       <c r="G17" s="99">
         <v>3</v>
       </c>
-      <c r="H17" s="119" t="s">
+      <c r="H17" s="118" t="s">
         <v>81</v>
       </c>
-      <c r="I17" s="119"/>
+      <c r="I17" s="118"/>
       <c r="J17" s="99">
         <v>4</v>
       </c>
@@ -5533,29 +5532,29 @@
       <c r="M17" s="99"/>
     </row>
     <row r="18" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="171">
-        <v>42736</v>
-      </c>
-      <c r="B18" s="171"/>
-      <c r="C18" s="119" t="s">
+      <c r="A18" s="170">
+        <v>42736</v>
+      </c>
+      <c r="B18" s="170"/>
+      <c r="C18" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="119" t="s">
+      <c r="D18" s="118" t="s">
         <v>232</v>
       </c>
-      <c r="E18" s="119" t="s">
+      <c r="E18" s="118" t="s">
         <v>84</v>
       </c>
-      <c r="F18" s="172" t="s">
+      <c r="F18" s="171" t="s">
         <v>235</v>
       </c>
       <c r="G18" s="99">
         <v>3</v>
       </c>
-      <c r="H18" s="119" t="s">
+      <c r="H18" s="118" t="s">
         <v>84</v>
       </c>
-      <c r="I18" s="119"/>
+      <c r="I18" s="118"/>
       <c r="J18" s="99">
         <v>5</v>
       </c>
@@ -5564,29 +5563,29 @@
       <c r="M18" s="99"/>
     </row>
     <row r="19" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="171">
-        <v>42736</v>
-      </c>
-      <c r="B19" s="171"/>
-      <c r="C19" s="119" t="s">
+      <c r="A19" s="170">
+        <v>42736</v>
+      </c>
+      <c r="B19" s="170"/>
+      <c r="C19" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="119" t="s">
+      <c r="D19" s="118" t="s">
         <v>232</v>
       </c>
-      <c r="E19" s="119" t="s">
+      <c r="E19" s="118" t="s">
         <v>85</v>
       </c>
-      <c r="F19" s="172" t="s">
+      <c r="F19" s="171" t="s">
         <v>235</v>
       </c>
       <c r="G19" s="99">
         <v>3</v>
       </c>
-      <c r="H19" s="119" t="s">
+      <c r="H19" s="118" t="s">
         <v>85</v>
       </c>
-      <c r="I19" s="119"/>
+      <c r="I19" s="118"/>
       <c r="J19" s="99">
         <v>6</v>
       </c>
@@ -5834,128 +5833,128 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="115" t="s">
+        <v>291</v>
+      </c>
+      <c r="B1" s="139" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="140" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="141" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="142" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="142" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="142" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="142" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" s="143" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="144" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="145" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="145" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4" s="124" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="124" t="s">
+        <v>293</v>
+      </c>
+      <c r="C4" s="124" t="s">
+        <v>295</v>
+      </c>
+      <c r="D4" s="124" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" s="124" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="124" t="s">
         <v>294</v>
       </c>
-      <c r="B1" s="140" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="141" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="142" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="143" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="143" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="143" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="143" t="s">
+      <c r="C5" s="124" t="s">
+        <v>297</v>
+      </c>
+      <c r="D5" s="124" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6" s="146" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="125" t="s">
+        <v>293</v>
+      </c>
+      <c r="C6" s="124" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="144" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="145" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="146" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="146" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="125" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="125" t="s">
+      <c r="D6" s="124" t="s">
         <v>296</v>
       </c>
-      <c r="C4" s="125" t="s">
-        <v>298</v>
-      </c>
-      <c r="D4" s="125" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A7" s="146" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="125" t="s">
+        <v>294</v>
+      </c>
+      <c r="C7" s="124" t="s">
+        <v>297</v>
+      </c>
+      <c r="D7" s="124" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A8" s="146" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="125" t="s">
+        <v>300</v>
+      </c>
+      <c r="C8" s="124" t="s">
+        <v>302</v>
+      </c>
+      <c r="D8" s="124" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A9" s="146" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="125" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="125" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="125" t="s">
-        <v>297</v>
-      </c>
-      <c r="C5" s="125" t="s">
-        <v>300</v>
-      </c>
-      <c r="D5" s="125" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="147" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="126" t="s">
-        <v>296</v>
-      </c>
-      <c r="C6" s="125" t="s">
-        <v>298</v>
-      </c>
-      <c r="D6" s="125" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="147" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="126" t="s">
-        <v>297</v>
-      </c>
-      <c r="C7" s="125" t="s">
-        <v>300</v>
-      </c>
-      <c r="D7" s="125" t="s">
+      <c r="C9" s="124" t="s">
+        <v>303</v>
+      </c>
+      <c r="D9" s="124" t="s">
         <v>304</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="147" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="126" t="s">
-        <v>303</v>
-      </c>
-      <c r="C8" s="125" t="s">
-        <v>305</v>
-      </c>
-      <c r="D8" s="125" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="147" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="126" t="s">
-        <v>302</v>
-      </c>
-      <c r="C9" s="125" t="s">
-        <v>306</v>
-      </c>
-      <c r="D9" s="125" t="s">
-        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -5968,7 +5967,7 @@
   <dimension ref="A1:IP12"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5981,17 +5980,17 @@
     <col min="251" max="1020" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:250" s="129" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="120" t="s">
+    <row r="1" spans="1:250" s="128" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="119" t="s">
         <v>244</v>
       </c>
-      <c r="B1" s="121" t="s">
+      <c r="B1" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="122" t="s">
+      <c r="C1" s="121" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="123" t="s">
+      <c r="D1" s="122" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="99"/>
@@ -6242,15 +6241,15 @@
       <c r="IP1" s="17"/>
     </row>
     <row r="2" spans="1:250" ht="65" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="127"/>
-      <c r="B2" s="127"/>
-      <c r="C2" s="128" t="s">
+      <c r="A2" s="126"/>
+      <c r="B2" s="126"/>
+      <c r="C2" s="127" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="128" t="s">
+      <c r="D2" s="127" t="s">
         <v>245</v>
       </c>
-      <c r="E2" s="128" t="s">
+      <c r="E2" s="127" t="s">
         <v>246</v>
       </c>
       <c r="F2" s="25"/>
@@ -6500,19 +6499,19 @@
       <c r="IP2" s="108"/>
     </row>
     <row r="3" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="124" t="s">
+      <c r="A3" s="123" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="124" t="s">
+      <c r="B3" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="148" t="s">
+      <c r="C3" s="147" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="149" t="s">
+      <c r="D3" s="148" t="s">
         <v>247</v>
       </c>
-      <c r="E3" s="124" t="s">
+      <c r="E3" s="123" t="s">
         <v>248</v>
       </c>
       <c r="F3" s="25"/>
@@ -6762,18 +6761,18 @@
       <c r="IP3" s="26"/>
     </row>
     <row r="4" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="118">
+      <c r="A4" s="117">
         <v>42736</v>
       </c>
       <c r="B4" s="99"/>
-      <c r="C4" s="119" t="s">
+      <c r="C4" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="150" t="s">
+      <c r="D4" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="E4" s="118" t="s">
         <v>249</v>
-      </c>
-      <c r="E4" s="119" t="s">
-        <v>250</v>
       </c>
       <c r="F4" s="25"/>
       <c r="G4" s="17"/>
@@ -7022,18 +7021,18 @@
       <c r="IP4" s="26"/>
     </row>
     <row r="5" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="118">
+      <c r="A5" s="117">
         <v>42736</v>
       </c>
       <c r="B5" s="99"/>
-      <c r="C5" s="119" t="s">
+      <c r="C5" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="119" t="s">
-        <v>251</v>
-      </c>
-      <c r="E5" s="119" t="s">
-        <v>252</v>
+      <c r="D5" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="E5" s="118" t="s">
+        <v>250</v>
       </c>
       <c r="F5" s="25"/>
       <c r="G5" s="17"/>
@@ -7282,17 +7281,17 @@
       <c r="IP5" s="26"/>
     </row>
     <row r="6" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="118">
+      <c r="A6" s="117">
         <v>42736</v>
       </c>
       <c r="B6" s="99"/>
-      <c r="C6" s="119" t="s">
+      <c r="C6" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="119" t="s">
-        <v>253</v>
-      </c>
-      <c r="E6" s="119" t="s">
+      <c r="D6" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="E6" s="118" t="s">
         <v>248</v>
       </c>
       <c r="F6" s="25"/>
@@ -7542,17 +7541,17 @@
       <c r="IP6" s="26"/>
     </row>
     <row r="7" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="118">
+      <c r="A7" s="117">
         <v>42736</v>
       </c>
       <c r="B7" s="99"/>
-      <c r="C7" s="119" t="s">
+      <c r="C7" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="125" t="s">
-        <v>297</v>
-      </c>
-      <c r="E7" s="119" t="s">
+      <c r="D7" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="E7" s="118" t="s">
         <v>248</v>
       </c>
       <c r="F7" s="25"/>
@@ -7802,18 +7801,18 @@
       <c r="IP7" s="108"/>
     </row>
     <row r="8" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="118">
+      <c r="A8" s="117">
         <v>42736</v>
       </c>
       <c r="B8" s="99"/>
-      <c r="C8" s="150" t="s">
+      <c r="C8" s="149" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="119" t="s">
-        <v>249</v>
-      </c>
-      <c r="E8" s="119" t="s">
-        <v>254</v>
+      <c r="D8" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="E8" s="118" t="s">
+        <v>251</v>
       </c>
       <c r="F8" s="25"/>
       <c r="G8" s="17"/>
@@ -8062,18 +8061,18 @@
       <c r="IP8" s="26"/>
     </row>
     <row r="9" spans="1:250" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="118">
+      <c r="A9" s="117">
         <v>42736</v>
       </c>
       <c r="B9" s="99"/>
-      <c r="C9" s="119" t="s">
+      <c r="C9" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="119" t="s">
-        <v>251</v>
-      </c>
-      <c r="E9" s="119" t="s">
-        <v>255</v>
+      <c r="D9" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="E9" s="118" t="s">
+        <v>252</v>
       </c>
       <c r="F9" s="25"/>
       <c r="G9" s="17"/>
@@ -8322,18 +8321,18 @@
       <c r="IP9" s="26"/>
     </row>
     <row r="10" spans="1:250" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="118">
+      <c r="A10" s="117">
         <v>42736</v>
       </c>
       <c r="B10" s="99"/>
-      <c r="C10" s="119" t="s">
+      <c r="C10" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="119" t="s">
+      <c r="D10" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="E10" s="118" t="s">
         <v>253</v>
-      </c>
-      <c r="E10" s="119" t="s">
-        <v>256</v>
       </c>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
@@ -8581,19 +8580,19 @@
       <c r="IO10" s="17"/>
       <c r="IP10" s="108"/>
     </row>
-    <row r="11" spans="1:250" s="129" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="118">
+    <row r="11" spans="1:250" s="128" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="117">
         <v>42736</v>
       </c>
       <c r="B11" s="99"/>
-      <c r="C11" s="119" t="s">
+      <c r="C11" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="126" t="s">
-        <v>302</v>
-      </c>
-      <c r="E11" s="119" t="s">
-        <v>256</v>
+      <c r="D11" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="E11" s="118" t="s">
+        <v>253</v>
       </c>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
@@ -8841,7 +8840,7 @@
       <c r="IO11" s="17"/>
       <c r="IP11" s="17"/>
     </row>
-    <row r="12" spans="1:250" s="129" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:250" s="128" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -9107,7 +9106,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9123,576 +9122,576 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="78" t="s">
-        <v>257</v>
-      </c>
-      <c r="B1" s="121" t="s">
+        <v>254</v>
+      </c>
+      <c r="B1" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="122" t="s">
+      <c r="C1" s="121" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="123" t="s">
+      <c r="D1" s="122" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
     </row>
     <row r="2" spans="1:6" ht="65" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="132"/>
-      <c r="B2" s="132"/>
-      <c r="C2" s="133" t="s">
+      <c r="A2" s="131"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="132" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="133" t="s">
+      <c r="D2" s="132" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="133" t="s">
+      <c r="E2" s="132" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="134" t="s">
+      <c r="F2" s="133" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="135" t="s">
+      <c r="A3" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="135" t="s">
+      <c r="B3" s="134" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="148" t="s">
+      <c r="C3" s="147" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="148" t="s">
+      <c r="D3" s="147" t="s">
         <v>193</v>
       </c>
-      <c r="E3" s="149" t="s">
+      <c r="E3" s="148" t="s">
         <v>247</v>
       </c>
-      <c r="F3" s="135" t="s">
+      <c r="F3" s="134" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="136">
-        <v>42736</v>
-      </c>
-      <c r="B4" s="131"/>
-      <c r="C4" s="130" t="s">
+      <c r="A4" s="135">
+        <v>42736</v>
+      </c>
+      <c r="B4" s="130"/>
+      <c r="C4" s="129" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="130" t="s">
+      <c r="D4" s="129" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="130" t="s">
+      <c r="E4" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F4" s="129" t="s">
         <v>249</v>
       </c>
-      <c r="F4" s="130" t="s">
+    </row>
+    <row r="5" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="135">
+        <v>42736</v>
+      </c>
+      <c r="B5" s="130"/>
+      <c r="C5" s="129" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="129" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F5" s="129" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="136">
-        <v>42736</v>
-      </c>
-      <c r="B5" s="131"/>
-      <c r="C5" s="130" t="s">
+    <row r="6" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="135">
+        <v>42736</v>
+      </c>
+      <c r="B6" s="130"/>
+      <c r="C6" s="129" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="130" t="s">
+      <c r="D6" s="129" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="130" t="s">
-        <v>251</v>
-      </c>
-      <c r="F5" s="130" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="136">
-        <v>42736</v>
-      </c>
-      <c r="B6" s="131"/>
-      <c r="C6" s="130" t="s">
+      <c r="E6" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F6" s="129" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="135">
+        <v>42736</v>
+      </c>
+      <c r="B7" s="130"/>
+      <c r="C7" s="129" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="130" t="s">
+      <c r="D7" s="129" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F7" s="129" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="135">
+        <v>42736</v>
+      </c>
+      <c r="B8" s="130"/>
+      <c r="C8" s="129" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="129" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F8" s="129" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="135">
+        <v>42736</v>
+      </c>
+      <c r="B9" s="130"/>
+      <c r="C9" s="129" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="129" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F9" s="129" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="136">
+        <v>42736</v>
+      </c>
+      <c r="B10" s="137"/>
+      <c r="C10" s="138" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="138" t="s">
+        <v>283</v>
+      </c>
+      <c r="E10" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F10" s="138" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="136">
+        <v>42736</v>
+      </c>
+      <c r="B11" s="137"/>
+      <c r="C11" s="138" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="118" t="s">
+        <v>279</v>
+      </c>
+      <c r="E11" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F11" s="138" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="136">
+        <v>42736</v>
+      </c>
+      <c r="B12" s="137"/>
+      <c r="C12" s="138" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="118" t="s">
+        <v>324</v>
+      </c>
+      <c r="E12" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F12" s="138" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="135">
+        <v>42736</v>
+      </c>
+      <c r="B13" s="130"/>
+      <c r="C13" s="129" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="129" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F13" s="129" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="135">
+        <v>42736</v>
+      </c>
+      <c r="B14" s="130"/>
+      <c r="C14" s="129" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="129" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F14" s="129" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="135">
+        <v>42736</v>
+      </c>
+      <c r="B15" s="130"/>
+      <c r="C15" s="129" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="129" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F15" s="129" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="135">
+        <v>42736</v>
+      </c>
+      <c r="B16" s="130"/>
+      <c r="C16" s="129" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="129" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F16" s="129" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="135">
+        <v>42736</v>
+      </c>
+      <c r="B17" s="130"/>
+      <c r="C17" s="129" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="129" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F17" s="129" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="135">
+        <v>42736</v>
+      </c>
+      <c r="B18" s="130"/>
+      <c r="C18" s="129" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="129" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F18" s="129" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="135">
+        <v>42736</v>
+      </c>
+      <c r="B19" s="130"/>
+      <c r="C19" s="129" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="129" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F19" s="129" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="135">
+        <v>42736</v>
+      </c>
+      <c r="B20" s="130"/>
+      <c r="C20" s="129" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="129" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="130" t="s">
-        <v>253</v>
-      </c>
-      <c r="F6" s="130" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="136">
-        <v>42736</v>
-      </c>
-      <c r="B7" s="131"/>
-      <c r="C7" s="130" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="130" t="s">
+      <c r="E20" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F20" s="129" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="135">
+        <v>42736</v>
+      </c>
+      <c r="B21" s="130"/>
+      <c r="C21" s="129" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="129" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="130" t="s">
+      <c r="E21" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F21" s="129" t="s">
         <v>249</v>
       </c>
-      <c r="F7" s="130" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="136">
-        <v>42736</v>
-      </c>
-      <c r="B8" s="131"/>
-      <c r="C8" s="130" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="130" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="130" t="s">
-        <v>251</v>
-      </c>
-      <c r="F8" s="130" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="136">
-        <v>42736</v>
-      </c>
-      <c r="B9" s="131"/>
-      <c r="C9" s="130" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="130" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="130" t="s">
-        <v>253</v>
-      </c>
-      <c r="F9" s="130" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="137">
-        <v>42736</v>
-      </c>
-      <c r="B10" s="138"/>
-      <c r="C10" s="139" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="139" t="s">
-        <v>286</v>
-      </c>
-      <c r="E10" s="139" t="s">
-        <v>253</v>
-      </c>
-      <c r="F10" s="139" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="137">
-        <v>42736</v>
-      </c>
-      <c r="B11" s="138"/>
-      <c r="C11" s="139" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="119" t="s">
-        <v>282</v>
-      </c>
-      <c r="E11" s="139" t="s">
-        <v>253</v>
-      </c>
-      <c r="F11" s="139" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="137">
-        <v>42736</v>
-      </c>
-      <c r="B12" s="138"/>
-      <c r="C12" s="139" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="119" t="s">
-        <v>327</v>
-      </c>
-      <c r="E12" s="139" t="s">
-        <v>253</v>
-      </c>
-      <c r="F12" s="139" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="136">
-        <v>42736</v>
-      </c>
-      <c r="B13" s="131"/>
-      <c r="C13" s="130" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="130" t="s">
+    </row>
+    <row r="22" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="135">
+        <v>42736</v>
+      </c>
+      <c r="B22" s="130"/>
+      <c r="C22" s="129" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="129" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="130" t="s">
+      <c r="E22" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F22" s="129" t="s">
         <v>249</v>
       </c>
-      <c r="F13" s="130" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="136">
-        <v>42736</v>
-      </c>
-      <c r="B14" s="131"/>
-      <c r="C14" s="130" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="130" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="130" t="s">
-        <v>251</v>
-      </c>
-      <c r="F14" s="130" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="136">
-        <v>42736</v>
-      </c>
-      <c r="B15" s="131"/>
-      <c r="C15" s="130" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="130" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="130" t="s">
-        <v>253</v>
-      </c>
-      <c r="F15" s="130" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="136">
-        <v>42736</v>
-      </c>
-      <c r="B16" s="131"/>
-      <c r="C16" s="130" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="130" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="130" t="s">
+    </row>
+    <row r="23" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="135">
+        <v>42736</v>
+      </c>
+      <c r="B23" s="130"/>
+      <c r="C23" s="129" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="129" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F23" s="129" t="s">
         <v>249</v>
       </c>
-      <c r="F16" s="130" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="136">
-        <v>42736</v>
-      </c>
-      <c r="B17" s="131"/>
-      <c r="C17" s="130" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="130" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="130" t="s">
+    </row>
+    <row r="24" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="135">
+        <v>42736</v>
+      </c>
+      <c r="B24" s="130"/>
+      <c r="C24" s="129" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="129" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F24" s="129" t="s">
         <v>249</v>
       </c>
-      <c r="F17" s="130" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="136">
-        <v>42736</v>
-      </c>
-      <c r="B18" s="131"/>
-      <c r="C18" s="130" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="130" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="130" t="s">
+    </row>
+    <row r="25" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="135">
+        <v>42736</v>
+      </c>
+      <c r="B25" s="130"/>
+      <c r="C25" s="129" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="129" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F25" s="129" t="s">
         <v>249</v>
       </c>
-      <c r="F18" s="130" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="136">
-        <v>42736</v>
-      </c>
-      <c r="B19" s="131"/>
-      <c r="C19" s="130" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="130" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="116" t="s">
-        <v>296</v>
-      </c>
-      <c r="F19" s="130" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="136">
-        <v>42736</v>
-      </c>
-      <c r="B20" s="131"/>
-      <c r="C20" s="130" t="s">
+    </row>
+    <row r="26" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="135">
+        <v>42736</v>
+      </c>
+      <c r="B26" s="130"/>
+      <c r="C26" s="129" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="130" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="130" t="s">
+      <c r="D26" s="129" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F26" s="129" t="s">
         <v>249</v>
       </c>
-      <c r="F20" s="130" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="136">
-        <v>42736</v>
-      </c>
-      <c r="B21" s="131"/>
-      <c r="C21" s="130" t="s">
+    </row>
+    <row r="27" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="135">
+        <v>42736</v>
+      </c>
+      <c r="B27" s="130"/>
+      <c r="C27" s="129" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="130" t="s">
-        <v>52</v>
-      </c>
-      <c r="E21" s="130" t="s">
+      <c r="D27" s="129" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F27" s="129" t="s">
         <v>249</v>
       </c>
-      <c r="F21" s="130" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="136">
-        <v>42736</v>
-      </c>
-      <c r="B22" s="131"/>
-      <c r="C22" s="130" t="s">
+    </row>
+    <row r="28" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="135">
+        <v>42736</v>
+      </c>
+      <c r="B28" s="130"/>
+      <c r="C28" s="129" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="130" t="s">
-        <v>54</v>
-      </c>
-      <c r="E22" s="130" t="s">
+      <c r="D28" s="129" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F28" s="129" t="s">
         <v>249</v>
       </c>
-      <c r="F22" s="130" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="136">
-        <v>42736</v>
-      </c>
-      <c r="B23" s="131"/>
-      <c r="C23" s="130" t="s">
+    </row>
+    <row r="29" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="135">
+        <v>42736</v>
+      </c>
+      <c r="B29" s="130"/>
+      <c r="C29" s="129" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="130" t="s">
-        <v>71</v>
-      </c>
-      <c r="E23" s="130" t="s">
+      <c r="D29" s="129" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F29" s="129" t="s">
         <v>249</v>
       </c>
-      <c r="F23" s="130" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="136">
-        <v>42736</v>
-      </c>
-      <c r="B24" s="131"/>
-      <c r="C24" s="130" t="s">
+    </row>
+    <row r="30" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="135">
+        <v>42736</v>
+      </c>
+      <c r="B30" s="130"/>
+      <c r="C30" s="129" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="130" t="s">
-        <v>74</v>
-      </c>
-      <c r="E24" s="130" t="s">
+      <c r="D30" s="129" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F30" s="129" t="s">
         <v>249</v>
       </c>
-      <c r="F24" s="130" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="136">
-        <v>42736</v>
-      </c>
-      <c r="B25" s="131"/>
-      <c r="C25" s="130" t="s">
+    </row>
+    <row r="31" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="135">
+        <v>42736</v>
+      </c>
+      <c r="B31" s="130"/>
+      <c r="C31" s="129" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="130" t="s">
-        <v>77</v>
-      </c>
-      <c r="E25" s="130" t="s">
+      <c r="D31" s="129" t="s">
+        <v>93</v>
+      </c>
+      <c r="E31" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F31" s="129" t="s">
         <v>249</v>
       </c>
-      <c r="F25" s="130" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="136">
-        <v>42736</v>
-      </c>
-      <c r="B26" s="131"/>
-      <c r="C26" s="130" t="s">
+    </row>
+    <row r="32" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="135">
+        <v>42736</v>
+      </c>
+      <c r="B32" s="130"/>
+      <c r="C32" s="129" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="130" t="s">
-        <v>79</v>
-      </c>
-      <c r="E26" s="130" t="s">
+      <c r="D32" s="129" t="s">
+        <v>96</v>
+      </c>
+      <c r="E32" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F32" s="129" t="s">
         <v>249</v>
-      </c>
-      <c r="F26" s="130" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="136">
-        <v>42736</v>
-      </c>
-      <c r="B27" s="131"/>
-      <c r="C27" s="130" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="130" t="s">
-        <v>81</v>
-      </c>
-      <c r="E27" s="130" t="s">
-        <v>249</v>
-      </c>
-      <c r="F27" s="130" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="136">
-        <v>42736</v>
-      </c>
-      <c r="B28" s="131"/>
-      <c r="C28" s="130" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="130" t="s">
-        <v>84</v>
-      </c>
-      <c r="E28" s="130" t="s">
-        <v>249</v>
-      </c>
-      <c r="F28" s="130" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="136">
-        <v>42736</v>
-      </c>
-      <c r="B29" s="131"/>
-      <c r="C29" s="130" t="s">
-        <v>27</v>
-      </c>
-      <c r="D29" s="130" t="s">
-        <v>85</v>
-      </c>
-      <c r="E29" s="130" t="s">
-        <v>249</v>
-      </c>
-      <c r="F29" s="130" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="136">
-        <v>42736</v>
-      </c>
-      <c r="B30" s="131"/>
-      <c r="C30" s="130" t="s">
-        <v>27</v>
-      </c>
-      <c r="D30" s="130" t="s">
-        <v>89</v>
-      </c>
-      <c r="E30" s="130" t="s">
-        <v>249</v>
-      </c>
-      <c r="F30" s="130" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="136">
-        <v>42736</v>
-      </c>
-      <c r="B31" s="131"/>
-      <c r="C31" s="130" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" s="130" t="s">
-        <v>93</v>
-      </c>
-      <c r="E31" s="130" t="s">
-        <v>249</v>
-      </c>
-      <c r="F31" s="130" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="136">
-        <v>42736</v>
-      </c>
-      <c r="B32" s="131"/>
-      <c r="C32" s="130" t="s">
-        <v>27</v>
-      </c>
-      <c r="D32" s="130" t="s">
-        <v>96</v>
-      </c>
-      <c r="E32" s="130" t="s">
-        <v>249</v>
-      </c>
-      <c r="F32" s="130" t="s">
-        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -9723,7 +9722,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -9750,10 +9749,10 @@
         <v>32</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -9768,16 +9767,16 @@
         <v>20</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>351</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>352</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>354</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="7"/>
@@ -9788,20 +9787,20 @@
       <c r="N3" s="8"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A4" s="117" t="s">
+      <c r="A4" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="117" t="s">
+      <c r="B4" s="116" t="s">
+        <v>353</v>
+      </c>
+      <c r="C4" s="199" t="s">
         <v>356</v>
       </c>
-      <c r="C4" s="201" t="s">
-        <v>359</v>
-      </c>
-      <c r="D4" s="201" t="s">
-        <v>357</v>
-      </c>
-      <c r="E4" s="200" t="s">
-        <v>358</v>
+      <c r="D4" s="199" t="s">
+        <v>354</v>
+      </c>
+      <c r="E4" s="198" t="s">
+        <v>355</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="3"/>
@@ -10030,173 +10029,176 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="6" max="6" width="13.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="185" t="s">
+      <c r="A1" s="184" t="s">
+        <v>334</v>
+      </c>
+      <c r="B1" s="185" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="186" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="187" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="188"/>
+      <c r="F1" s="188"/>
+      <c r="G1" s="188"/>
+    </row>
+    <row r="2" spans="1:7" ht="252" x14ac:dyDescent="0.15">
+      <c r="A2" s="189"/>
+      <c r="B2" s="189"/>
+      <c r="C2" s="190" t="s">
+        <v>335</v>
+      </c>
+      <c r="D2" s="190" t="s">
+        <v>336</v>
+      </c>
+      <c r="E2" s="190" t="s">
         <v>337</v>
       </c>
-      <c r="B1" s="186" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="187" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="188" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="189"/>
-      <c r="F1" s="189"/>
-      <c r="G1" s="189"/>
-    </row>
-    <row r="2" spans="1:7" ht="252" x14ac:dyDescent="0.15">
-      <c r="A2" s="190"/>
-      <c r="B2" s="190"/>
-      <c r="C2" s="191" t="s">
+      <c r="F2" s="190" t="s">
         <v>338</v>
       </c>
-      <c r="D2" s="191" t="s">
+      <c r="G2" s="190" t="s">
         <v>339</v>
       </c>
-      <c r="E2" s="191" t="s">
-        <v>340</v>
-      </c>
-      <c r="F2" s="191" t="s">
-        <v>341</v>
-      </c>
-      <c r="G2" s="191" t="s">
-        <v>342</v>
-      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="192" t="s">
+      <c r="A3" s="191" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="192" t="s">
+      <c r="B3" s="191" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="193" t="s">
+      <c r="C3" s="192" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="193" t="s">
+      <c r="D3" s="192" t="s">
         <v>193</v>
       </c>
-      <c r="E3" s="193" t="s">
+      <c r="E3" s="192" t="s">
         <v>99</v>
       </c>
-      <c r="F3" s="192" t="s">
+      <c r="F3" s="191" t="s">
         <v>247</v>
       </c>
-      <c r="G3" s="192" t="s">
+      <c r="G3" s="191" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="194">
-        <v>42736</v>
-      </c>
-      <c r="B4" s="189"/>
-      <c r="C4" s="195" t="s">
+      <c r="A4" s="193">
+        <v>42736</v>
+      </c>
+      <c r="B4" s="188"/>
+      <c r="C4" s="194" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="196" t="s">
+      <c r="D4" s="195" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="196" t="s">
+      <c r="E4" s="195" t="s">
         <v>119</v>
       </c>
-      <c r="F4" s="197" t="s">
+      <c r="F4" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="G4" s="188" t="s">
         <v>249</v>
       </c>
-      <c r="G4" s="189" t="s">
-        <v>250</v>
-      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="194">
-        <v>42736</v>
-      </c>
-      <c r="B5" s="189"/>
-      <c r="C5" s="195" t="s">
+      <c r="A5" s="193">
+        <v>42736</v>
+      </c>
+      <c r="B5" s="188"/>
+      <c r="C5" s="194" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="196" t="s">
+      <c r="D5" s="195" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="196" t="s">
+      <c r="E5" s="195" t="s">
         <v>121</v>
       </c>
-      <c r="F5" s="197" t="s">
+      <c r="F5" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="G5" s="188" t="s">
         <v>249</v>
       </c>
-      <c r="G5" s="189" t="s">
-        <v>250</v>
-      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="194">
-        <v>42736</v>
-      </c>
-      <c r="B6" s="189"/>
-      <c r="C6" s="195" t="s">
+      <c r="A6" s="193">
+        <v>42736</v>
+      </c>
+      <c r="B6" s="188"/>
+      <c r="C6" s="194" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="196" t="s">
+      <c r="D6" s="195" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="196" t="s">
+      <c r="E6" s="195" t="s">
         <v>123</v>
       </c>
-      <c r="F6" s="197" t="s">
+      <c r="F6" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="G6" s="188" t="s">
         <v>249</v>
       </c>
-      <c r="G6" s="189" t="s">
-        <v>250</v>
-      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" s="194">
-        <v>42736</v>
-      </c>
-      <c r="B7" s="189"/>
-      <c r="C7" s="195" t="s">
+      <c r="A7" s="193">
+        <v>42736</v>
+      </c>
+      <c r="B7" s="188"/>
+      <c r="C7" s="194" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="196" t="s">
+      <c r="D7" s="195" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="196" t="s">
+      <c r="E7" s="195" t="s">
         <v>125</v>
       </c>
-      <c r="F7" s="197" t="s">
+      <c r="F7" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="G7" s="188" t="s">
         <v>249</v>
       </c>
-      <c r="G7" s="189" t="s">
-        <v>250</v>
-      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="194">
-        <v>42736</v>
-      </c>
-      <c r="B8" s="189"/>
-      <c r="C8" s="195" t="s">
+      <c r="A8" s="193">
+        <v>42736</v>
+      </c>
+      <c r="B8" s="188"/>
+      <c r="C8" s="194" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="196" t="s">
+      <c r="D8" s="195" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="196" t="s">
+      <c r="E8" s="195" t="s">
         <v>126</v>
       </c>
-      <c r="F8" s="197" t="s">
+      <c r="F8" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="G8" s="188" t="s">
         <v>249</v>
-      </c>
-      <c r="G8" s="189" t="s">
-        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -10208,7 +10210,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:IU15"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -10222,7 +10226,7 @@
   <sheetData>
     <row r="1" spans="1:255" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -10495,7 +10499,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>246</v>
@@ -11030,11 +11034,11 @@
       <c r="D4" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>249</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>250</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -11297,11 +11301,11 @@
       <c r="D5" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>251</v>
+      <c r="E5" s="212" t="s">
+        <v>369</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -11564,11 +11568,11 @@
       <c r="D6" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>253</v>
+      <c r="E6" s="212" t="s">
+        <v>369</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -11831,11 +11835,11 @@
       <c r="D7" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>253</v>
+      <c r="E7" s="212" t="s">
+        <v>369</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -12098,11 +12102,11 @@
       <c r="D8" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>249</v>
+      <c r="E8" s="212" t="s">
+        <v>369</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -12365,11 +12369,11 @@
       <c r="D9" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>251</v>
+      <c r="E9" s="212" t="s">
+        <v>369</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -12632,11 +12636,11 @@
       <c r="D10" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>249</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>250</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
@@ -12899,11 +12903,11 @@
       <c r="D11" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>251</v>
+      <c r="E11" s="212" t="s">
+        <v>369</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -13166,11 +13170,11 @@
       <c r="D12" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>253</v>
+      <c r="E12" s="212" t="s">
+        <v>369</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
@@ -13433,11 +13437,11 @@
       <c r="D13" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>253</v>
+      <c r="E13" s="212" t="s">
+        <v>369</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
@@ -13700,11 +13704,11 @@
       <c r="D14" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>249</v>
+      <c r="E14" s="212" t="s">
+        <v>369</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
@@ -13967,11 +13971,11 @@
       <c r="D15" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>251</v>
+      <c r="E15" s="212" t="s">
+        <v>369</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -14237,7 +14241,7 @@
   <dimension ref="A1:IU15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -14252,7 +14256,7 @@
   <sheetData>
     <row r="1" spans="1:255" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="80" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B1" s="81" t="s">
         <v>1</v>
@@ -14525,7 +14529,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="89" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F2" s="89" t="s">
         <v>246</v>
@@ -14549,7 +14553,7 @@
         <v>36</v>
       </c>
       <c r="D3" s="93" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E3" s="93" t="s">
         <v>247</v>
@@ -14576,11 +14580,11 @@
       <c r="D4" s="95" t="s">
         <v>145</v>
       </c>
-      <c r="E4" s="95" t="s">
+      <c r="E4" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F4" s="95" t="s">
         <v>249</v>
-      </c>
-      <c r="F4" s="95" t="s">
-        <v>250</v>
       </c>
       <c r="G4" s="84"/>
       <c r="H4" s="84"/>
@@ -14601,11 +14605,11 @@
       <c r="D5" s="95" t="s">
         <v>145</v>
       </c>
-      <c r="E5" s="95" t="s">
-        <v>253</v>
+      <c r="E5" s="212" t="s">
+        <v>369</v>
       </c>
       <c r="F5" s="95" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G5" s="84"/>
       <c r="H5" s="84"/>
@@ -14626,11 +14630,11 @@
       <c r="D6" s="95" t="s">
         <v>147</v>
       </c>
-      <c r="E6" s="95" t="s">
-        <v>249</v>
+      <c r="E6" s="212" t="s">
+        <v>369</v>
       </c>
       <c r="F6" s="95" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G6" s="84"/>
       <c r="H6" s="84"/>
@@ -14651,11 +14655,11 @@
       <c r="D7" s="95" t="s">
         <v>147</v>
       </c>
-      <c r="E7" s="95" t="s">
-        <v>251</v>
+      <c r="E7" s="212" t="s">
+        <v>369</v>
       </c>
       <c r="F7" s="95" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G7" s="84"/>
       <c r="H7" s="84"/>
@@ -14676,11 +14680,11 @@
       <c r="D8" s="95" t="s">
         <v>149</v>
       </c>
-      <c r="E8" s="95" t="s">
-        <v>251</v>
+      <c r="E8" s="212" t="s">
+        <v>369</v>
       </c>
       <c r="F8" s="95" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G8" s="84"/>
       <c r="H8" s="84"/>
@@ -14701,11 +14705,11 @@
       <c r="D9" s="95" t="s">
         <v>149</v>
       </c>
-      <c r="E9" s="95" t="s">
-        <v>253</v>
+      <c r="E9" s="212" t="s">
+        <v>369</v>
       </c>
       <c r="F9" s="95" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G9" s="84"/>
       <c r="H9" s="84"/>
@@ -14726,11 +14730,11 @@
       <c r="D10" s="95" t="s">
         <v>145</v>
       </c>
-      <c r="E10" s="95" t="s">
+      <c r="E10" s="212" t="s">
+        <v>369</v>
+      </c>
+      <c r="F10" s="95" t="s">
         <v>249</v>
-      </c>
-      <c r="F10" s="95" t="s">
-        <v>250</v>
       </c>
       <c r="G10" s="84"/>
       <c r="H10" s="84"/>
@@ -14751,11 +14755,11 @@
       <c r="D11" s="95" t="s">
         <v>145</v>
       </c>
-      <c r="E11" s="95" t="s">
-        <v>253</v>
+      <c r="E11" s="212" t="s">
+        <v>369</v>
       </c>
       <c r="F11" s="95" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G11" s="84"/>
       <c r="H11" s="84"/>
@@ -14776,11 +14780,11 @@
       <c r="D12" s="95" t="s">
         <v>147</v>
       </c>
-      <c r="E12" s="95" t="s">
-        <v>249</v>
+      <c r="E12" s="212" t="s">
+        <v>369</v>
       </c>
       <c r="F12" s="95" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G12" s="84"/>
       <c r="H12" s="84"/>
@@ -14801,11 +14805,11 @@
       <c r="D13" s="95" t="s">
         <v>147</v>
       </c>
-      <c r="E13" s="95" t="s">
-        <v>251</v>
+      <c r="E13" s="212" t="s">
+        <v>369</v>
       </c>
       <c r="F13" s="95" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G13" s="84"/>
       <c r="H13" s="84"/>
@@ -14826,11 +14830,11 @@
       <c r="D14" s="95" t="s">
         <v>149</v>
       </c>
-      <c r="E14" s="95" t="s">
-        <v>251</v>
+      <c r="E14" s="212" t="s">
+        <v>369</v>
       </c>
       <c r="F14" s="95" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G14" s="84"/>
       <c r="H14" s="84"/>
@@ -14851,11 +14855,11 @@
       <c r="D15" s="95" t="s">
         <v>149</v>
       </c>
-      <c r="E15" s="95" t="s">
-        <v>253</v>
+      <c r="E15" s="212" t="s">
+        <v>369</v>
       </c>
       <c r="F15" s="95" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G15" s="84"/>
       <c r="H15" s="84"/>
@@ -15120,8 +15124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -15132,82 +15136,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="156" t="s">
+      <c r="A1" s="155" t="s">
+        <v>317</v>
+      </c>
+      <c r="B1" s="156" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="157" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="158" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="84" x14ac:dyDescent="0.15">
+      <c r="A2" s="159"/>
+      <c r="B2" s="159" t="s">
+        <v>318</v>
+      </c>
+      <c r="C2" s="159" t="s">
+        <v>319</v>
+      </c>
+      <c r="D2" s="159"/>
+    </row>
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="160" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="160" t="s">
         <v>320</v>
       </c>
-      <c r="B1" s="157" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="158" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="159" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="84" x14ac:dyDescent="0.15">
-      <c r="A2" s="160"/>
-      <c r="B2" s="160" t="s">
+      <c r="C3" s="160" t="s">
+        <v>193</v>
+      </c>
+      <c r="D3" s="160"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4" s="161" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="124" t="s">
         <v>321</v>
       </c>
-      <c r="C2" s="160" t="s">
+      <c r="C4" s="124" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="162"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" s="161" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="124" t="s">
+        <v>321</v>
+      </c>
+      <c r="C5" s="124" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="162"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6" s="161" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="162" t="s">
         <v>322</v>
       </c>
-      <c r="D2" s="160"/>
-    </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="161" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="161" t="s">
+      <c r="C6" s="124" t="s">
         <v>323</v>
       </c>
-      <c r="C3" s="161" t="s">
-        <v>193</v>
-      </c>
-      <c r="D3" s="161"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="162" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="125" t="s">
-        <v>324</v>
-      </c>
-      <c r="C4" s="125" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="163"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="162" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="125" t="s">
-        <v>324</v>
-      </c>
-      <c r="C5" s="125" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="163"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="162" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="163" t="s">
-        <v>325</v>
-      </c>
-      <c r="C6" s="125" t="s">
-        <v>326</v>
-      </c>
-      <c r="D6" s="163"/>
+      <c r="D6" s="162"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="163"/>
-      <c r="B7" s="163"/>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
+      <c r="A7" s="162"/>
+      <c r="B7" s="162"/>
+      <c r="C7" s="162"/>
+      <c r="D7" s="162"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15601,7 +15605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E882E8-CCDE-8C41-B416-088AC35BA427}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+    <sheetView zoomScale="112" workbookViewId="0">
       <selection sqref="A1:C7"/>
     </sheetView>
   </sheetViews>
@@ -15614,58 +15618,58 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3" ht="28" x14ac:dyDescent="0.15">
-      <c r="A2" s="206" t="s">
+      <c r="A2" s="204" t="s">
+        <v>363</v>
+      </c>
+      <c r="B2" s="204" t="s">
         <v>366</v>
       </c>
-      <c r="B2" s="206" t="s">
-        <v>369</v>
-      </c>
-      <c r="C2" s="206" t="s">
-        <v>370</v>
+      <c r="C2" s="204" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.15">
-      <c r="A3" s="207" t="s">
-        <v>366</v>
-      </c>
-      <c r="B3" s="208" t="s">
-        <v>367</v>
-      </c>
-      <c r="C3" s="209" t="s">
+      <c r="A3" s="205" t="s">
+        <v>363</v>
+      </c>
+      <c r="B3" s="206" t="s">
+        <v>364</v>
+      </c>
+      <c r="C3" s="207" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.15">
+      <c r="A4" s="208" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.15">
-      <c r="A4" s="210" t="s">
-        <v>371</v>
-      </c>
-      <c r="B4" s="210" t="s">
+      <c r="B4" s="208" t="s">
         <v>176</v>
       </c>
-      <c r="C4" s="211" t="s">
+      <c r="C4" s="209" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.15">
-      <c r="A5" s="210"/>
-      <c r="B5" s="210"/>
-      <c r="C5" s="211"/>
+      <c r="A5" s="208"/>
+      <c r="B5" s="208"/>
+      <c r="C5" s="209"/>
     </row>
     <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.15">
-      <c r="A6" s="210"/>
-      <c r="B6" s="212"/>
-      <c r="C6" s="213"/>
+      <c r="A6" s="208"/>
+      <c r="B6" s="210"/>
+      <c r="C6" s="211"/>
     </row>
     <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.15">
-      <c r="A7" s="210"/>
-      <c r="B7" s="210"/>
-      <c r="C7" s="211"/>
+      <c r="A7" s="208"/>
+      <c r="B7" s="208"/>
+      <c r="C7" s="209"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15679,7 +15683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W42"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="H2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -16216,14 +16220,14 @@
         <v>24</v>
       </c>
       <c r="D14" s="112" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="E14" s="111" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="F14" s="113"/>
       <c r="G14" s="111" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="H14" s="113"/>
       <c r="I14" s="113"/>
@@ -16253,14 +16257,14 @@
         <v>24</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F15" s="99"/>
       <c r="G15" s="3" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="H15" s="99"/>
       <c r="I15" s="99"/>
@@ -16290,14 +16294,14 @@
         <v>24</v>
       </c>
       <c r="D16" s="33" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="E16" s="34" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F16" s="99"/>
       <c r="G16" s="3" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="H16" s="99"/>
       <c r="I16" s="99"/>
@@ -16326,17 +16330,17 @@
       <c r="C17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="117" t="s">
-        <v>316</v>
-      </c>
-      <c r="E17" s="117" t="s">
-        <v>317</v>
+      <c r="D17" s="116" t="s">
+        <v>313</v>
+      </c>
+      <c r="E17" s="116" t="s">
+        <v>314</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="H17" s="117" t="s">
+      <c r="H17" s="116" t="s">
         <v>95</v>
       </c>
       <c r="I17" s="4"/>
@@ -16362,76 +16366,76 @@
         <v>42736</v>
       </c>
       <c r="B18" s="109"/>
-      <c r="C18" s="178" t="s">
+      <c r="C18" s="177" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="179" t="s">
-        <v>332</v>
-      </c>
-      <c r="E18" s="179" t="s">
-        <v>333</v>
-      </c>
-      <c r="F18" s="180"/>
-      <c r="G18" s="178" t="s">
-        <v>334</v>
-      </c>
-      <c r="H18" s="179"/>
-      <c r="I18" s="180"/>
-      <c r="J18" s="180"/>
-      <c r="K18" s="178" t="s">
+      <c r="D18" s="178" t="s">
+        <v>329</v>
+      </c>
+      <c r="E18" s="178" t="s">
+        <v>330</v>
+      </c>
+      <c r="F18" s="179"/>
+      <c r="G18" s="177" t="s">
+        <v>331</v>
+      </c>
+      <c r="H18" s="178"/>
+      <c r="I18" s="179"/>
+      <c r="J18" s="179"/>
+      <c r="K18" s="177" t="s">
         <v>26</v>
       </c>
-      <c r="L18" s="180"/>
-      <c r="M18" s="180"/>
-      <c r="N18" s="180"/>
-      <c r="O18" s="180"/>
-      <c r="P18" s="180"/>
-      <c r="Q18" s="180"/>
-      <c r="R18" s="180"/>
-      <c r="S18" s="181"/>
-      <c r="T18" s="182"/>
-      <c r="U18" s="182"/>
-      <c r="V18" s="182"/>
-      <c r="W18" s="183"/>
+      <c r="L18" s="179"/>
+      <c r="M18" s="179"/>
+      <c r="N18" s="179"/>
+      <c r="O18" s="179"/>
+      <c r="P18" s="179"/>
+      <c r="Q18" s="179"/>
+      <c r="R18" s="179"/>
+      <c r="S18" s="180"/>
+      <c r="T18" s="181"/>
+      <c r="U18" s="181"/>
+      <c r="V18" s="181"/>
+      <c r="W18" s="182"/>
     </row>
     <row r="19" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="109">
         <v>42736</v>
       </c>
       <c r="B19" s="109"/>
-      <c r="C19" s="178" t="s">
+      <c r="C19" s="177" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="179" t="s">
-        <v>335</v>
-      </c>
-      <c r="E19" s="179" t="s">
-        <v>336</v>
-      </c>
-      <c r="F19" s="180"/>
-      <c r="G19" s="178" t="s">
-        <v>334</v>
-      </c>
-      <c r="H19" s="178" t="s">
+      <c r="D19" s="178" t="s">
+        <v>332</v>
+      </c>
+      <c r="E19" s="178" t="s">
+        <v>333</v>
+      </c>
+      <c r="F19" s="179"/>
+      <c r="G19" s="177" t="s">
+        <v>331</v>
+      </c>
+      <c r="H19" s="177" t="s">
         <v>88</v>
       </c>
-      <c r="I19" s="180"/>
-      <c r="J19" s="180"/>
-      <c r="K19" s="178" t="s">
+      <c r="I19" s="179"/>
+      <c r="J19" s="179"/>
+      <c r="K19" s="177" t="s">
         <v>26</v>
       </c>
-      <c r="L19" s="180"/>
-      <c r="M19" s="180"/>
-      <c r="N19" s="180"/>
-      <c r="O19" s="180"/>
-      <c r="P19" s="180"/>
-      <c r="Q19" s="180"/>
-      <c r="R19" s="180"/>
-      <c r="S19" s="181"/>
-      <c r="T19" s="182"/>
-      <c r="U19" s="182"/>
-      <c r="V19" s="182"/>
-      <c r="W19" s="183"/>
+      <c r="L19" s="179"/>
+      <c r="M19" s="179"/>
+      <c r="N19" s="179"/>
+      <c r="O19" s="179"/>
+      <c r="P19" s="179"/>
+      <c r="Q19" s="179"/>
+      <c r="R19" s="179"/>
+      <c r="S19" s="180"/>
+      <c r="T19" s="181"/>
+      <c r="U19" s="181"/>
+      <c r="V19" s="181"/>
+      <c r="W19" s="182"/>
     </row>
     <row r="20" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="9">
@@ -17190,7 +17194,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -17258,7 +17262,7 @@
       <c r="E3" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="F3" s="184" t="s">
+      <c r="F3" s="183" t="s">
         <v>144</v>
       </c>
       <c r="G3" s="8"/>
@@ -17547,7 +17551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -17616,8 +17620,8 @@
       <c r="G2" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="H2" s="198" t="s">
-        <v>343</v>
+      <c r="H2" s="196" t="s">
+        <v>340</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>35</v>
@@ -17664,7 +17668,7 @@
       <c r="G3" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="H3" s="199" t="s">
+      <c r="H3" s="197" t="s">
         <v>144</v>
       </c>
       <c r="I3" s="7" t="s">
@@ -17712,8 +17716,8 @@
         <v>120</v>
       </c>
       <c r="G4" s="3"/>
-      <c r="H4" s="150" t="s">
-        <v>346</v>
+      <c r="H4" s="149" t="s">
+        <v>343</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -17748,8 +17752,8 @@
         <v>122</v>
       </c>
       <c r="G5" s="3"/>
-      <c r="H5" s="150" t="s">
-        <v>347</v>
+      <c r="H5" s="149" t="s">
+        <v>344</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -17784,8 +17788,8 @@
         <v>124</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="150" t="s">
-        <v>348</v>
+      <c r="H6" s="149" t="s">
+        <v>345</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -17820,8 +17824,8 @@
         <v>125</v>
       </c>
       <c r="G7" s="3"/>
-      <c r="H7" s="150" t="s">
-        <v>344</v>
+      <c r="H7" s="149" t="s">
+        <v>341</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -17858,8 +17862,8 @@
       <c r="G8" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="H8" s="150" t="s">
-        <v>345</v>
+      <c r="H8" s="149" t="s">
+        <v>342</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -17894,7 +17898,7 @@
         <v>128</v>
       </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="119"/>
+      <c r="H9" s="118"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -17928,7 +17932,7 @@
         <v>46</v>
       </c>
       <c r="G10" s="3"/>
-      <c r="H10" s="119"/>
+      <c r="H10" s="118"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -17962,7 +17966,7 @@
         <v>131</v>
       </c>
       <c r="G11" s="3"/>
-      <c r="H11" s="119"/>
+      <c r="H11" s="118"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
@@ -17996,7 +18000,7 @@
         <v>53</v>
       </c>
       <c r="G12" s="3"/>
-      <c r="H12" s="119"/>
+      <c r="H12" s="118"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -18030,7 +18034,7 @@
         <v>133</v>
       </c>
       <c r="G13" s="3"/>
-      <c r="H13" s="119"/>
+      <c r="H13" s="118"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
@@ -18064,7 +18068,7 @@
         <v>135</v>
       </c>
       <c r="G14" s="3"/>
-      <c r="H14" s="119"/>
+      <c r="H14" s="118"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -18098,7 +18102,7 @@
         <v>10</v>
       </c>
       <c r="G15" s="3"/>
-      <c r="H15" s="119"/>
+      <c r="H15" s="118"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
@@ -18132,7 +18136,7 @@
         <v>138</v>
       </c>
       <c r="G16" s="3"/>
-      <c r="H16" s="119"/>
+      <c r="H16" s="118"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
@@ -18166,7 +18170,7 @@
         <v>140</v>
       </c>
       <c r="G17" s="3"/>
-      <c r="H17" s="119"/>
+      <c r="H17" s="118"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
@@ -18200,7 +18204,7 @@
         <v>10</v>
       </c>
       <c r="G18" s="3"/>
-      <c r="H18" s="119"/>
+      <c r="H18" s="118"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
@@ -18234,7 +18238,7 @@
         <v>138</v>
       </c>
       <c r="G19" s="3"/>
-      <c r="H19" s="119"/>
+      <c r="H19" s="118"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
@@ -18268,7 +18272,7 @@
         <v>140</v>
       </c>
       <c r="G20" s="3"/>
-      <c r="H20" s="119"/>
+      <c r="H20" s="118"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -18897,7 +18901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="E1" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C3" sqref="C3:E3"/>
     </sheetView>
   </sheetViews>
@@ -19007,13 +19011,13 @@
         <v>160</v>
       </c>
       <c r="R2" s="103" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="S2" s="106" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="T2" s="106" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="U2" s="5"/>
     </row>
@@ -19070,13 +19074,13 @@
         <v>169</v>
       </c>
       <c r="R3" s="104" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="S3" s="107" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="T3" s="107" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="U3" s="8"/>
     </row>
@@ -19105,10 +19109,10 @@
         <v>145</v>
       </c>
       <c r="J4" s="41" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="K4" s="41" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="L4" s="41"/>
       <c r="M4" s="41"/>
@@ -19124,7 +19128,7 @@
         <v>172</v>
       </c>
       <c r="S4" s="99" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="T4" s="99" t="s">
         <v>172</v>
@@ -19173,7 +19177,7 @@
         <v>176</v>
       </c>
       <c r="S5" s="99" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="T5" s="99"/>
       <c r="U5" s="4"/>

</xml_diff>